<commit_message>
Update WES template example to pass validations
</commit_message>
<xml_diff>
--- a/template_examples/wes.xlsx
+++ b/template_examples/wes.xlsx
@@ -1,25 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/template_examples/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9126B1F0-DDE7-7A43-9332-2D873A9D7AB4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="21260" windowHeight="13040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WES" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -32,7 +38,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -45,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -58,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -71,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -84,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -97,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -110,12 +116,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -123,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -136,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0">
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -149,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0">
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -162,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C14" authorId="0">
+    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -175,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D14" authorId="0">
+    <comment ref="D14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -188,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E14" authorId="0">
+    <comment ref="E14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -201,7 +207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="0">
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -214,7 +220,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G14" authorId="0">
+    <comment ref="G14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -227,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H14" authorId="0">
+    <comment ref="H14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -240,7 +246,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I14" authorId="0">
+    <comment ref="I14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -253,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J14" authorId="0">
+    <comment ref="J14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -266,7 +272,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K14" authorId="0">
+    <comment ref="K14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -279,7 +285,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L14" authorId="0">
+    <comment ref="L14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
@@ -292,7 +298,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M14" authorId="0">
+    <comment ref="M14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
       <text>
         <r>
           <rPr>
@@ -310,7 +316,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="41">
   <si>
     <t>#t</t>
   </si>
@@ -394,13 +400,52 @@
   </si>
   <si>
     <t>READ GROUP MAPPING FILE</t>
+  </si>
+  <si>
+    <t>DFCI</t>
+  </si>
+  <si>
+    <t>Agilent</t>
+  </si>
+  <si>
+    <t>Human All Exon V7</t>
+  </si>
+  <si>
+    <t>KAPA</t>
+  </si>
+  <si>
+    <t>Hyper Prep</t>
+  </si>
+  <si>
+    <t>Illumina</t>
+  </si>
+  <si>
+    <t>HiSeq 2500</t>
+  </si>
+  <si>
+    <t>Paired</t>
+  </si>
+  <si>
+    <t>CIMAC-12309</t>
+  </si>
+  <si>
+    <t>CIMAC-432123</t>
+  </si>
+  <si>
+    <t>asfasdf.q</t>
+  </si>
+  <si>
+    <t>fdsafdsa.q</t>
+  </si>
+  <si>
+    <t>asdf.asdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,18 +454,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -489,22 +540,30 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -551,7 +610,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -583,9 +642,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -617,6 +694,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -792,1279 +887,1337 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="101" width="30.7109375" customWidth="1"/>
+    <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+    </row>
+    <row r="2" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="C5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="C8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="C9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="C10" s="1">
+        <v>100</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="B13" s="2" t="s">
+      <c r="C11" s="1">
+        <v>1230912309</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="L14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="M14" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15">
+        <v>123</v>
+      </c>
+      <c r="E15">
+        <v>321</v>
+      </c>
+      <c r="F15" s="4">
+        <v>41193</v>
+      </c>
+      <c r="G15" s="4">
+        <v>41193</v>
+      </c>
+      <c r="H15">
+        <v>10</v>
+      </c>
+      <c r="I15">
+        <v>5</v>
+      </c>
+      <c r="J15">
+        <v>5</v>
+      </c>
+      <c r="K15" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15" t="s">
+        <v>39</v>
+      </c>
+      <c r="M15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:1">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:1">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:1">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:1">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="113" spans="1:1">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:1">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:1">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:1">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:1">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="118" spans="1:1">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="1:1">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="1:1">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="121" spans="1:1">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="1:1">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:1">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="124" spans="1:1">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="125" spans="1:1">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="1:1">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="1:1">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:1">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="1:1">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="130" spans="1:1">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:1">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="132" spans="1:1">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="133" spans="1:1">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="134" spans="1:1">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="135" spans="1:1">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="136" spans="1:1">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="137" spans="1:1">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="139" spans="1:1">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="140" spans="1:1">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="141" spans="1:1">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="142" spans="1:1">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="143" spans="1:1">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="144" spans="1:1">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="145" spans="1:1">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="146" spans="1:1">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="147" spans="1:1">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="148" spans="1:1">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="149" spans="1:1">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="150" spans="1:1">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="151" spans="1:1">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:1">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:1">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:1">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="156" spans="1:1">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="157" spans="1:1">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="158" spans="1:1">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="160" spans="1:1">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="161" spans="1:1">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="162" spans="1:1">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="163" spans="1:1">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="164" spans="1:1">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="165" spans="1:1">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="166" spans="1:1">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="167" spans="1:1">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="168" spans="1:1">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="169" spans="1:1">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="170" spans="1:1">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="171" spans="1:1">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="172" spans="1:1">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="173" spans="1:1">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="174" spans="1:1">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="175" spans="1:1">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="176" spans="1:1">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="177" spans="1:1">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="178" spans="1:1">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="179" spans="1:1">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="180" spans="1:1">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="181" spans="1:1">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="182" spans="1:1">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="183" spans="1:1">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="184" spans="1:1">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="185" spans="1:1">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="186" spans="1:1">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="187" spans="1:1">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="188" spans="1:1">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="189" spans="1:1">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="190" spans="1:1">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="191" spans="1:1">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="192" spans="1:1">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="193" spans="1:1">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="194" spans="1:1">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="195" spans="1:1">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="196" spans="1:1">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="197" spans="1:1">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="198" spans="1:1">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="199" spans="1:1">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="200" spans="1:1">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="201" spans="1:1">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="202" spans="1:1">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="203" spans="1:1">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="204" spans="1:1">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="205" spans="1:1">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="206" spans="1:1">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="207" spans="1:1">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="208" spans="1:1">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="209" spans="1:1">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="210" spans="1:1">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="211" spans="1:1">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="212" spans="1:1">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="213" spans="1:1">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="214" spans="1:1">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>15</v>
       </c>
@@ -2075,11 +2228,11 @@
     <mergeCell ref="B13:M13"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="F15:F214">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>"Paired,Single"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="F15:G214" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>AND(ISNUMBER(F15:F214),LEFT(CELL("format",F15:F214),1)="D")</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="G15:G214">
-      <formula1>AND(ISNUMBER(G15:G214),LEFT(CELL("format",G15:G214),1)="D")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix WES and add RNA for expression datamodel and templates (#33)
</commit_message>
<xml_diff>
--- a/template_examples/wes.xlsx
+++ b/template_examples/wes.xlsx
@@ -1,31 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27715"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/md299/PycharmProjects/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9126B1F0-DDE7-7A43-9332-2D873A9D7AB4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="21260" windowHeight="13040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12060" yWindow="460" windowWidth="30480" windowHeight="14160"/>
   </bookViews>
   <sheets>
     <sheet name="WES" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -38,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -51,20 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>The version of the bait set used, e.g. Human All Exon V7</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="B4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -77,33 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>The version of the library construction kit used, e.g. Hyper Prep</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sequencing Platform, eg. Illumina, IonTorrent</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -116,12 +84,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="B6" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -129,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="B7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -142,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="B8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -155,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="B11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -168,7 +136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="C11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -181,7 +149,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="D14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="D11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The type of material submitted - tumor/normal/etc</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -194,7 +175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="F11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -207,7 +188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="G11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -220,7 +201,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+    <comment ref="H11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -233,7 +214,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+    <comment ref="I11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -242,11 +223,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Amount of DNA (in ng) used for library construction</t>
+          <t>Amount of DNA/RNA (in ng) used for library construction</t>
         </r>
       </text>
     </comment>
-    <comment ref="I14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="J11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -259,7 +240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="K11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -272,7 +253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+    <comment ref="L11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -281,11 +262,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Fastq file for the forward read</t>
+          <t>Fastq file for the forward reads</t>
         </r>
       </text>
     </comment>
-    <comment ref="L14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
+    <comment ref="M11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -294,11 +275,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Fastq file for the reverse read</t>
+          <t>Fastq file for the reverse reads</t>
         </r>
       </text>
     </comment>
-    <comment ref="M14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
+    <comment ref="N11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -316,7 +297,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="45">
   <si>
     <t>#t</t>
   </si>
@@ -330,24 +311,15 @@
     <t>CREATOR</t>
   </si>
   <si>
-    <t>BAIT VENDOR</t>
-  </si>
-  <si>
-    <t>BAIT VERSION</t>
+    <t>ENRICHMENT KIT</t>
   </si>
   <si>
     <t>LIBRARY KIT VENDOR</t>
   </si>
   <si>
-    <t>LIBRARY KIT VERSION</t>
-  </si>
-  <si>
     <t>SEQUENCER PLATFORM</t>
   </si>
   <si>
-    <t>SEQUENCER MODEL</t>
-  </si>
-  <si>
     <t>PAIRED END READS</t>
   </si>
   <si>
@@ -372,10 +344,13 @@
     <t>CIMAC ALIQUOT ID</t>
   </si>
   <si>
+    <t>GENOMIC SOURCE</t>
+  </si>
+  <si>
     <t>LIBRARY KIT LOT</t>
   </si>
   <si>
-    <t>BAIT LOT</t>
+    <t>ENRICHMENT LOT</t>
   </si>
   <si>
     <t>LIBRARY PREP DATE</t>
@@ -402,50 +377,68 @@
     <t>READ GROUP MAPPING FILE</t>
   </si>
   <si>
-    <t>DFCI</t>
-  </si>
-  <si>
-    <t>Agilent</t>
-  </si>
-  <si>
-    <t>Human All Exon V7</t>
-  </si>
-  <si>
-    <t>KAPA</t>
-  </si>
-  <si>
-    <t>Hyper Prep</t>
-  </si>
-  <si>
-    <t>Illumina</t>
-  </si>
-  <si>
-    <t>HiSeq 2500</t>
+    <t>Broad Institute</t>
+  </si>
+  <si>
+    <t>Agilent - Human All Exon V7</t>
+  </si>
+  <si>
+    <t>KAPA - Hyper Prep</t>
+  </si>
+  <si>
+    <t>Illumina - NovaSeq 6000</t>
   </si>
   <si>
     <t>Paired</t>
   </si>
   <si>
-    <t>CIMAC-12309</t>
-  </si>
-  <si>
-    <t>CIMAC-432123</t>
-  </si>
-  <si>
-    <t>asfasdf.q</t>
-  </si>
-  <si>
-    <t>fdsafdsa.q</t>
-  </si>
-  <si>
-    <t>asdf.asdf</t>
+    <t>Study 1</t>
+  </si>
+  <si>
+    <t>Patient 1</t>
+  </si>
+  <si>
+    <t>aliquot1</t>
+  </si>
+  <si>
+    <t>Tumor</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>eafgh</t>
+  </si>
+  <si>
+    <t>gs://path/to/fwd.fastq</t>
+  </si>
+  <si>
+    <t>gs://path/to/rev.fastq</t>
+  </si>
+  <si>
+    <t>gs://path/to/read_group.map</t>
+  </si>
+  <si>
+    <t>aliquot2</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>gs://path/to/fwd2.fastq</t>
+  </si>
+  <si>
+    <t>gs://path/to/rev2.fastq</t>
+  </si>
+  <si>
+    <t>gs://path/to/read_group2.map</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -464,12 +457,6 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -560,9 +547,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -613,9 +597,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -643,31 +627,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -695,23 +662,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -887,11 +837,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M214"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -900,7 +850,7 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -918,8 +868,9 @@
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
-    </row>
-    <row r="2" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -927,7 +878,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -939,8 +890,9 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -948,7 +900,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -960,8 +912,9 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -969,7 +922,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -981,8 +934,9 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -990,7 +944,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1002,8 +956,9 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1011,7 +966,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1023,16 +978,17 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>33</v>
+      <c r="C7" s="1">
+        <v>100</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1044,8 +1000,9 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1053,7 +1010,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1065,1174 +1022,1173 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="N8" s="1"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="1">
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="4">
+        <v>43586</v>
+      </c>
+      <c r="H12" s="4">
+        <v>43587</v>
+      </c>
+      <c r="I12">
+        <v>200</v>
+      </c>
+      <c r="J12">
+        <v>760</v>
+      </c>
+      <c r="K12">
+        <v>250</v>
+      </c>
+      <c r="L12" t="s">
+        <v>37</v>
+      </c>
+      <c r="M12" t="s">
+        <v>38</v>
+      </c>
+      <c r="N12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="4">
+        <v>43586</v>
+      </c>
+      <c r="H13" s="4">
+        <v>43587</v>
+      </c>
+      <c r="I13">
         <v>100</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1230912309</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <v>450</v>
+      </c>
+      <c r="K13">
+        <v>200</v>
+      </c>
+      <c r="L13" t="s">
+        <v>42</v>
+      </c>
+      <c r="M13" t="s">
+        <v>43</v>
+      </c>
+      <c r="N13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15">
-        <v>123</v>
-      </c>
-      <c r="E15">
-        <v>321</v>
-      </c>
-      <c r="F15" s="4">
-        <v>41193</v>
-      </c>
-      <c r="G15" s="4">
-        <v>41193</v>
-      </c>
-      <c r="H15">
-        <v>10</v>
-      </c>
-      <c r="I15">
-        <v>5</v>
-      </c>
-      <c r="J15">
-        <v>5</v>
-      </c>
-      <c r="K15" t="s">
-        <v>38</v>
-      </c>
-      <c r="L15" t="s">
-        <v>39</v>
-      </c>
-      <c r="M15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A212" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A213" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A214" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:M1"/>
-    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B1:N1"/>
+    <mergeCell ref="B10:N10"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
+      <formula1>"Agilent - Human All Exon V7,Twist,IDT,NEB"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
+      <formula1>"KAPA - Hyper Prep"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
+      <formula1>"Illumina - HiSeq 2500,Illumina - HiSeq 3000,Illumina - NextSeq 550,Illumina - HiSeq 4000,Illumina - NovaSeq 6000"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6">
       <formula1>"Paired,Single"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="F15:G214" xr:uid="{00000000-0002-0000-0000-000001000000}">
-      <formula1>AND(ISNUMBER(F15:F214),LEFT(CELL("format",F15:F214),1)="D")</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12:D211">
+      <formula1>"Tumor,Normal,Metastasis"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="G12:G211">
+      <formula1>AND(ISNUMBER(G12:G211),LEFT(CELL("format",G12:G211),1)="D")</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="H12:H211">
+      <formula1>AND(ISNUMBER(H12:H211),LEFT(CELL("format",H12:H211),1)="D")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>